<commit_message>
Updating processed words in Vocabulary.xlsx
</commit_message>
<xml_diff>
--- a/Vocabulary.xlsx
+++ b/Vocabulary.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
   <si>
     <t>word</t>
   </si>
@@ -814,6 +814,9 @@
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="C18" t="s" s="0">
+        <v>71</v>
+      </c>
     </row>
     <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -822,6 +825,9 @@
       <c r="B19" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C19" t="s" s="0">
+        <v>71</v>
+      </c>
     </row>
     <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -830,6 +836,9 @@
       <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="C20" t="s" s="0">
+        <v>71</v>
+      </c>
     </row>
     <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -838,6 +847,9 @@
       <c r="B21" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="C21" t="s" s="0">
+        <v>71</v>
+      </c>
     </row>
     <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -845,6 +857,9 @@
       </c>
       <c r="B22" s="1" t="s">
         <v>44</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated processed vocabulary rows
</commit_message>
<xml_diff>
--- a/Vocabulary.xlsx
+++ b/Vocabulary.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2480" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2490" uniqueCount="88">
   <si>
     <t>word</t>
   </si>
@@ -727,6 +727,9 @@
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C6" t="s" s="0">
+        <v>87</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -735,6 +738,9 @@
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C7" t="s" s="0">
+        <v>87</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -743,6 +749,9 @@
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C8" t="s" s="0">
+        <v>87</v>
+      </c>
     </row>
     <row r="9" spans="1:2" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -751,6 +760,9 @@
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C9" t="s" s="0">
+        <v>87</v>
+      </c>
     </row>
     <row r="10" spans="1:2" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -758,6 +770,9 @@
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>